<commit_message>
Updated Again To Be Safe
I updated this 10 minutes ago, and then I closed the sheet. It asked if I wanted to save changes. I did, and am now uploading it again just to be safe.
</commit_message>
<xml_diff>
--- a/Scoring Re-Check.xlsx
+++ b/Scoring Re-Check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ziako\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52BAC16B-F4F7-4485-9683-B6714B4EBA5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C49AFE-FBD4-406E-9D2D-A77A76B498E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="46" r:id="rId6"/>
+    <pivotCache cacheId="56" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -3300,7 +3300,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="ziako" refreshedDate="43993.594904050929" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="920" xr:uid="{B3513818-0BD5-4D44-A7E5-BA4C27A08656}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="ziako" refreshedDate="43993.61852708333" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="920" xr:uid="{B3513818-0BD5-4D44-A7E5-BA4C27A08656}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:AA1048576" sheet="Totals"/>
   </cacheSource>
@@ -30706,7 +30706,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{667F8EFB-DD0A-4C84-B905-6BE5F7BDB603}" name="PivotTable1" cacheId="46" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="5" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{667F8EFB-DD0A-4C84-B905-6BE5F7BDB603}" name="PivotTable1" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="5" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A17:Q461" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="31">
     <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -32656,7 +32656,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{65148AAA-4F0D-4D67-A93C-FB77EAFA6608}" name="PivotTable2" cacheId="46" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{65148AAA-4F0D-4D67-A93C-FB77EAFA6608}" name="PivotTable2" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A5:R7" firstHeaderRow="0" firstDataRow="1" firstDataCol="2" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="31">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -33269,7 +33269,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8987A1B2-596C-49A5-A957-B1F5A93D07C4}" name="PivotTable1" cacheId="46" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8987A1B2-596C-49A5-A957-B1F5A93D07C4}" name="PivotTable1" cacheId="56" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A4:B20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="31">
     <pivotField showAll="0"/>
@@ -33468,7 +33468,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{625F5DE7-DBC5-42C1-AF24-0FBF55523329}" name="PivotTable1" cacheId="46" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="5" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{625F5DE7-DBC5-42C1-AF24-0FBF55523329}" name="PivotTable1" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="5" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A4:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="31">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -34333,8 +34333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB920"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A429" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="74" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A411" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
@@ -60421,7 +60421,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>